<commit_message>
added trigger for delta load; convert draws to numeric
</commit_message>
<xml_diff>
--- a/Data_Gathering/Results_default.xlsx
+++ b/Data_Gathering/Results_default.xlsx
@@ -489,35 +489,23 @@
           <t>37-32-02-22-03-20</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>37</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="C2" t="n">
+        <v>37</v>
+      </c>
+      <c r="D2" t="n">
+        <v>32</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>22</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="3">

</xml_diff>